<commit_message>
point to graph and stocks
</commit_message>
<xml_diff>
--- a/rendements_et_risques.xlsx
+++ b/rendements_et_risques.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,75 +452,322 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.001965916502864335</v>
+        <v>0.000409195432119712</v>
       </c>
       <c r="C2" t="n">
-        <v>0.02330636580045176</v>
+        <v>0.01577304597325203</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>AI.PA</t>
+          <t>ADA-USD</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0005630637044797611</v>
+        <v>0.002109322907709398</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01493207543416745</v>
+        <v>0.05385911692947309</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>GOOGL</t>
+          <t>AMZN</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.001651575163367829</v>
+        <v>-6.331447102676818e-05</v>
       </c>
       <c r="C4" t="n">
-        <v>0.02000694397426247</v>
+        <v>0.0197547657637857</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>MC.PA</t>
+          <t>BABA</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.001317171046907658</v>
+        <v>-0.0006555208053647794</v>
       </c>
       <c r="C5" t="n">
-        <v>0.01925130228065546</v>
+        <v>0.02917146136629337</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>MSFT</t>
+          <t>BNB-USD</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.001696231832603212</v>
+        <v>0.003300274737707548</v>
       </c>
       <c r="C6" t="n">
-        <v>0.02140726355664707</v>
+        <v>0.05275003261595376</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>TSLA</t>
+          <t>BTC-USD</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.005928016706353079</v>
+        <v>0.001338890310131067</v>
       </c>
       <c r="C7" t="n">
-        <v>0.04625324658590867</v>
+        <v>0.03414030084679871</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>DAI-USD</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-2.317790536334618e-05</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.002147598150660589</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>DOGE-USD</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.007118002616628462</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1316804669561277</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>DOT-USD</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.001307446046721384</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.05807611652739767</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>ETH-USD</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.002288183890886724</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.0450493043897679</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>GOOG</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.0005561434150984816</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.01657202065415029</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.0005525675125263694</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.01659933490063376</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>JNJ</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>8.346392399517444e-05</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.008663813227800198</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>JPM</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.0004363184681520799</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.01386509989112363</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>MATIC-USD</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.005231289252545505</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.07498958764790675</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.0004038578094758204</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.01497815621918233</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>SOL-USD</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.004044725884465609</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.07182484297952729</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>TON-USD</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.0006277791916024</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.06824254427809426</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>TRX-USD</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0.002231566251630027</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.04737623518475711</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>USDC-USD</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-1.439140654660258e-06</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.001241952029302097</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>USDT-USD</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-2.050810642745787e-06</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.0007281035275920827</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.000151766101611962</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.01318653829784571</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>VOD</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>-0.0002438401746817289</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.014529915233304</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>WBTC-USD</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.001281691832933432</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.03417820766614947</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>XRP-USD</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0.002536448557910965</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.06508533059648003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>